<commit_message>
added correct descriptive network results
</commit_message>
<xml_diff>
--- a/output-descriptive analysis/general-descriptive-analysis/General descriptive analysis.xlsx
+++ b/output-descriptive analysis/general-descriptive-analysis/General descriptive analysis.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thesis/Desktop/Google Drive/thesis-lorenz/Data-handling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thesis/Desktop/Google Drive/thesis-lorenz/Supplementary material thesis/output-descriptive-analysis/general-descriptive-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Species</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -158,7 +161,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -277,8 +280,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -294,20 +326,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -316,7 +342,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -327,8 +352,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -336,6 +369,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -343,9 +377,56 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="25">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -483,6 +564,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -492,13 +580,6 @@
         <top style="thin">
           <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -590,9 +671,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -707,28 +785,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
@@ -740,43 +796,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A9:F12" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A9:F12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A7:F10" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="A7:F10"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Species" dataDxfId="21"/>
-    <tableColumn id="2" name="# unique GO labels" dataDxfId="20"/>
-    <tableColumn id="3" name="range of # labels/pathogen protein" dataDxfId="19"/>
-    <tableColumn id="4" name="Avg # labels/pathogen protein" dataDxfId="18"/>
-    <tableColumn id="5" name="range of # labels/human protein" dataDxfId="17"/>
-    <tableColumn id="6" name="Avg # labels/human protein" dataDxfId="16"/>
+    <tableColumn id="1" name="Species" dataDxfId="24"/>
+    <tableColumn id="2" name="# unique GO labels" dataDxfId="23"/>
+    <tableColumn id="3" name="range of # labels/pathogen protein" dataDxfId="22"/>
+    <tableColumn id="4" name="Avg # labels/pathogen protein" dataDxfId="21"/>
+    <tableColumn id="5" name="range of # labels/human protein" dataDxfId="20"/>
+    <tableColumn id="6" name="Avg # labels/human protein" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A14:F17" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A14:F17" totalsRowShown="0" headerRowDxfId="0" dataDxfId="18" headerRowBorderDxfId="1">
   <autoFilter ref="A14:F17"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Species" dataDxfId="13"/>
-    <tableColumn id="2" name="# unique IPR labels" dataDxfId="12"/>
-    <tableColumn id="3" name="range of # labels/pathogen protein" dataDxfId="11"/>
-    <tableColumn id="4" name="Avg # labels/pathogen protein" dataDxfId="10"/>
-    <tableColumn id="5" name="range of # labels/human protein" dataDxfId="9"/>
-    <tableColumn id="6" name="Avg # labels/human protein" dataDxfId="8"/>
+    <tableColumn id="1" name="Species" dataDxfId="17"/>
+    <tableColumn id="2" name="# unique IPR labels" dataDxfId="16"/>
+    <tableColumn id="3" name="range of # labels/pathogen protein" dataDxfId="15"/>
+    <tableColumn id="4" name="Avg # labels/pathogen protein" dataDxfId="14"/>
+    <tableColumn id="5" name="range of # labels/human protein" dataDxfId="13"/>
+    <tableColumn id="6" name="Avg # labels/human protein" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="G1:J4" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="G1:J4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table42" displayName="Table42" ref="A1:D4" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:D4"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Species" dataDxfId="3"/>
-    <tableColumn id="2" name="# pathogen proteins" dataDxfId="2"/>
-    <tableColumn id="3" name="# human proteins" dataDxfId="1"/>
-    <tableColumn id="4" name="# interactions" dataDxfId="0"/>
+    <tableColumn id="1" name="Species" dataDxfId="7"/>
+    <tableColumn id="2" name="# pathogen proteins" dataDxfId="6"/>
+    <tableColumn id="3" name="# human proteins" dataDxfId="5"/>
+    <tableColumn id="4" name="# interactions" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1048,14 +1104,14 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
@@ -1066,251 +1122,266 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G2" s="17" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="12">
+      <c r="B2" s="4">
         <v>346</v>
       </c>
-      <c r="I2" s="12">
+      <c r="C2" s="4">
         <v>982</v>
       </c>
-      <c r="J2" s="18">
+      <c r="D2" s="9">
         <v>1335</v>
       </c>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G3" s="17" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="12">
+      <c r="B3" s="4">
         <v>942</v>
       </c>
-      <c r="I3" s="12">
+      <c r="C3" s="4">
         <v>1713</v>
       </c>
-      <c r="J3" s="18">
+      <c r="D3" s="9">
         <v>3185</v>
       </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G4" s="19" t="s">
+      <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="15">
+      <c r="B4" s="7">
         <v>1223</v>
       </c>
-      <c r="I4" s="15">
+      <c r="C4" s="7">
         <v>2149</v>
       </c>
-      <c r="J4" s="20">
+      <c r="D4" s="11">
         <v>4098</v>
       </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="5"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G6" s="16"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="8"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G8" s="9"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="11"/>
-    </row>
-    <row r="9" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="21"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+    </row>
+    <row r="7" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="21"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+    </row>
+    <row r="8" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="12">
+        <v>5907</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="12">
+        <v>7.34</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="12">
+        <v>25.87</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="14"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="12">
+        <v>7609</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="12">
+        <v>5.7</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="12">
+        <v>25.86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="12">
+        <v>8899</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="12">
+        <v>6.18</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="12">
+        <v>26.34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="13" t="s">
+      <c r="B14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F14" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
+    <row r="15" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="21">
-        <v>5907</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="21">
-        <v>7.34</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="21">
-        <v>25.87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
+      <c r="B15" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="12">
+        <v>6.1</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="12">
+        <v>4.84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="21">
-        <v>7609</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="21">
-        <v>5.7</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="21">
-        <v>25.86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
+      <c r="B16" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="12">
+        <v>4.26</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="12">
+        <v>5.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="21">
-        <v>8899</v>
-      </c>
-      <c r="C12" s="21" t="s">
+      <c r="B17" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="21">
-        <v>6.18</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="21">
-        <v>26.34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="21">
-        <v>6.1</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="21">
-        <v>4.84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="21">
-        <v>4.26</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="21">
-        <v>5.01</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="21">
+      <c r="D17" s="12">
         <v>4.66</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="12">
         <v>5.17</v>
       </c>
     </row>

</xml_diff>